<commit_message>
Game broke - fixed & implemented sounds
</commit_message>
<xml_diff>
--- a/Audio_Asset_Sheet.xlsx
+++ b/Audio_Asset_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\GitHub\ct5034-platformer-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B35BAE-AADE-470D-A4AA-700ADF2AA5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA1C70-7B1D-4681-8ACA-D2344838F285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Original Assets Used</t>
   </si>
@@ -87,16 +87,9 @@
     <t>e.g.</t>
   </si>
   <si>
-    <t>1. LowPass used to remove bass tones to produce a tinny zapping tone. 
-2. Automation on volume used linked to ammo count to change sound when ammo is low.</t>
-  </si>
-  <si>
     <t>FMOD Event Name</t>
   </si>
   <si>
-    <t>PlayerLaserRifle</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
@@ -109,16 +102,6 @@
     <t>FMOD Effects Used</t>
   </si>
   <si>
-    <t>1. Scatterer Sound
-2. Volume Automation
-3. 3D Spatializer</t>
-  </si>
-  <si>
-    <t>1. "WeirdScifiSound" - freesound.org/weirdscifisound
-2. "ZapZap" - airbournesound.com/scifisounds
-3. "Click" - freesound.org/click001</t>
-  </si>
-  <si>
     <t>DAW Effects Used</t>
   </si>
   <si>
@@ -126,9 +109,6 @@
   </si>
   <si>
     <t>UE4 Trigger</t>
-  </si>
-  <si>
-    <t>Triggers when the player fires the Laser Rifle weapon.</t>
   </si>
   <si>
     <t>CT5034 Asset Sheet - Assignment 1</t>
@@ -151,11 +131,6 @@
   </si>
   <si>
     <t>Platformer</t>
-  </si>
-  <si>
-    <t>1. Audacity: bass boost EQ and slow speed for intended gun sound.
-2. Abelton MIDI keyboard &amp; instruments for various ambiance.
-3. Transposed "enginerev" to sound like a different vehicle.</t>
   </si>
   <si>
     <t>Wheel Spin</t>
@@ -174,6 +149,12 @@
   </si>
   <si>
     <t>1. Reduced gap between squeaks - increase tempo.</t>
+  </si>
+  <si>
+    <t>1. Audacity: bass boost EQ and slow speed for intended gun sound.
+2. Abelton MIDI keyboard &amp; instruments for various ambiance.
+3. Transposed "enginerev" to sound like a different vehicle.
+4. Used panning automation on each car sound</t>
   </si>
 </sst>
 </file>
@@ -237,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,6 +317,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,13 +351,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>179294</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>627530</xdr:rowOff>
+      <xdr:rowOff>743814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2066617</xdr:colOff>
+      <xdr:colOff>1937106</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1669676</xdr:rowOff>
+      <xdr:rowOff>1669675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -390,8 +387,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1141319" y="1932455"/>
-          <a:ext cx="3944723" cy="1042146"/>
+          <a:off x="1142496" y="2038786"/>
+          <a:ext cx="3502279" cy="925861"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -480,7 +477,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1455506</xdr:colOff>
+      <xdr:colOff>1455507</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>21405</xdr:rowOff>
     </xdr:to>
@@ -865,48 +862,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" customWidth="1"/>
+    <col min="7" max="7" width="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" s="5"/>
       <c r="E2" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -918,25 +915,25 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -944,19 +941,17 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -964,37 +959,24 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="F9" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1157,14 +1139,14 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
+      <c r="B27" s="18">
         <v>20</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="10">

</xml_diff>